<commit_message>
Fills out day planner for the entire day
</commit_message>
<xml_diff>
--- a/backend/uploaded_templates/Empty.xlsx
+++ b/backend/uploaded_templates/Empty.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28512"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="577" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0DE1D5B-37BA-44AC-B3E8-81CE0CE13AC2}"/>
+  <xr:revisionPtr revIDLastSave="579" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F3EF197-BE89-442C-BEC4-005F6143FA02}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -705,7 +705,7 @@
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>